<commit_message>
version-gen-test add case:no tags test
</commit_message>
<xml_diff>
--- a/build-version/version-gen-case/version-gen-case.xlsx
+++ b/build-version/version-gen-case/version-gen-case.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>本地是否有修改</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -228,6 +228,16 @@
   </si>
   <si>
     <t>..\version-gen-test\test-10.PNG</t>
+  </si>
+  <si>
+    <t>报错</t>
+  </si>
+  <si>
+    <t>报错</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>..\version-gen-test\test-11.PNG</t>
   </si>
 </sst>
 </file>
@@ -271,12 +281,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -296,7 +312,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -319,6 +335,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -776,7 +801,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1069,21 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -1072,6 +1111,7 @@
     <hyperlink ref="G9" r:id="rId8"/>
     <hyperlink ref="G10" r:id="rId9"/>
     <hyperlink ref="G11" r:id="rId10"/>
+    <hyperlink ref="G12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>